<commit_message>
Classifier coding and more
</commit_message>
<xml_diff>
--- a/CountryIndexes/DB_SupplyChain_MA.xlsx
+++ b/CountryIndexes/DB_SupplyChain_MA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yassinezahrouni/coding/test/CountryIndexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D50A30-5144-744B-9228-78089808BB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4C5D16-C9B5-5546-BB35-869B6E44F090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="38400" windowHeight="21120" activeTab="5" xr2:uid="{63F6B712-49FA-2545-A479-242A3D2165A0}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="38400" windowHeight="21120" activeTab="8" xr2:uid="{63F6B712-49FA-2545-A479-242A3D2165A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview Itinerary Part" sheetId="1" r:id="rId1"/>
@@ -43265,8 +43265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C96E0F-6F5A-E341-A6C7-770A83D51C58}">
   <dimension ref="A1:J954"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A251" workbookViewId="0">
-      <selection activeCell="C681" sqref="C681"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -65394,8 +65394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3793894-AE5F-AA41-A6F7-73672CEC5B4D}">
   <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>